<commit_message>
Added data for 2017 profiles, fixed spelling in raw data, all tests passed.
</commit_message>
<xml_diff>
--- a/raw/MajorEmployers 2017.xlsx
+++ b/raw/MajorEmployers 2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="685">
   <si>
     <t xml:space="preserve">Date Received</t>
   </si>
@@ -1493,7 +1493,7 @@
     <t xml:space="preserve">Stonington</t>
   </si>
   <si>
-    <t xml:space="preserve">David Standard LLC</t>
+    <t xml:space="preserve">Davis Standard LLC</t>
   </si>
   <si>
     <t xml:space="preserve">McQuades Market Inc.</t>
@@ -2025,9 +2025,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nustone MFG + Distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Davis Standard LLC</t>
   </si>
   <si>
     <t xml:space="preserve">LCS Westminster Partnership</t>
@@ -2225,17 +2222,17 @@
   </sheetPr>
   <dimension ref="A1:L170"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C147" activeCellId="0" sqref="C147"/>
+      <selection pane="bottomLeft" activeCell="C138" activeCellId="0" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5171,22 +5168,22 @@
   </sheetPr>
   <dimension ref="A1:K170"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E156" activeCellId="0" sqref="E156"/>
+      <selection pane="bottomLeft" activeCell="B138" activeCellId="0" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6741,10 +6738,10 @@
         <v>489</v>
       </c>
       <c r="B138" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D138" s="0" t="s">
         <v>668</v>
-      </c>
-      <c r="D138" s="0" t="s">
-        <v>669</v>
       </c>
       <c r="F138" s="0" t="s">
         <v>492</v>
@@ -6899,19 +6896,19 @@
         <v>543</v>
       </c>
       <c r="B151" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="D151" s="0" t="s">
         <v>670</v>
       </c>
-      <c r="D151" s="0" t="s">
+      <c r="F151" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="F151" s="0" t="s">
+      <c r="H151" s="0" t="s">
         <v>672</v>
       </c>
-      <c r="H151" s="0" t="s">
+      <c r="J151" s="0" t="s">
         <v>673</v>
-      </c>
-      <c r="J151" s="0" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6973,13 +6970,13 @@
         <v>558</v>
       </c>
       <c r="F155" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="H155" s="0" t="s">
         <v>675</v>
       </c>
-      <c r="H155" s="0" t="s">
+      <c r="J155" s="0" t="s">
         <v>676</v>
-      </c>
-      <c r="J155" s="0" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7010,16 +7007,16 @@
         <v>570</v>
       </c>
       <c r="D157" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="F157" s="0" t="s">
         <v>678</v>
       </c>
-      <c r="F157" s="0" t="s">
+      <c r="H157" s="0" t="s">
         <v>679</v>
       </c>
-      <c r="H157" s="0" t="s">
+      <c r="J157" s="0" t="s">
         <v>680</v>
-      </c>
-      <c r="J157" s="0" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7096,7 +7093,7 @@
         <v>65</v>
       </c>
       <c r="J161" s="0" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7159,7 +7156,7 @@
         <v>606</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D164" s="0" t="s">
         <v>608</v>
@@ -7208,7 +7205,7 @@
         <v>628</v>
       </c>
       <c r="E169" s="0" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F169" s="0" t="s">
         <v>629</v>
@@ -7223,7 +7220,7 @@
         <v>63</v>
       </c>
       <c r="J169" s="0" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="K169" s="0" t="n">
         <v>30</v>

</xml_diff>